<commit_message>
Startup with bibs displayed
</commit_message>
<xml_diff>
--- a/dummy data.xlsx
+++ b/dummy data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\tryoutTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD00B05A-67C5-4780-AD86-7A33B6903FDE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{A836094F-D8AD-434F-B4E5-A0112D063DBB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="2" xr2:uid="{A836094F-D8AD-434F-B4E5-A0112D063DBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -18,7 +19,7 @@
   </sheets>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -3459,7 +3460,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7DFA8D81-0FB9-4498-B220-A5DBD4A1D2C2}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7DFA8D81-0FB9-4498-B220-A5DBD4A1D2C2}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" showAll="0"/>
@@ -3891,7 +3892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAE72A7-7AE9-4E6B-BD02-33690A7E1982}">
   <dimension ref="A3:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -4086,7 +4087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE802AE-603D-41B8-B2C4-3FDD5CDA8C14}">
   <dimension ref="A1:M321"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A280" workbookViewId="0">
       <selection activeCell="C312" sqref="A2:G321"/>
     </sheetView>
   </sheetViews>
@@ -11819,8 +11820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AA0ED0-D424-46CC-B0C8-45FC504602F3}">
   <dimension ref="A1:A500"/>
   <sheetViews>
-    <sheetView topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="A166" sqref="A166"/>
+    <sheetView tabSelected="1" topLeftCell="A282" workbookViewId="0">
+      <selection activeCell="A316" sqref="A316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13749,1084 +13750,544 @@
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A321" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D322, "',",Players!A322, ",'",Players!E322,"','",Players!F322,"','",Players!G322,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A321" s="2"/>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D323, "',",Players!A323, ",'",Players!E323,"','",Players!F323,"','",Players!G323,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A322" s="2"/>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A323" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D324, "',",Players!A324, ",'",Players!E324,"','",Players!F324,"','",Players!G324,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A323" s="2"/>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A324" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D325, "',",Players!A325, ",'",Players!E325,"','",Players!F325,"','",Players!G325,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A324" s="2"/>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A325" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D326, "',",Players!A326, ",'",Players!E326,"','",Players!F326,"','",Players!G326,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A325" s="2"/>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A326" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D327, "',",Players!A327, ",'",Players!E327,"','",Players!F327,"','",Players!G327,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A326" s="2"/>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A327" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D328, "',",Players!A328, ",'",Players!E328,"','",Players!F328,"','",Players!G328,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A327" s="2"/>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A328" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D329, "',",Players!A329, ",'",Players!E329,"','",Players!F329,"','",Players!G329,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A328" s="2"/>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A329" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D330, "',",Players!A330, ",'",Players!E330,"','",Players!F330,"','",Players!G330,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A329" s="2"/>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A330" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D331, "',",Players!A331, ",'",Players!E331,"','",Players!F331,"','",Players!G331,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A330" s="2"/>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A331" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D332, "',",Players!A332, ",'",Players!E332,"','",Players!F332,"','",Players!G332,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A331" s="2"/>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A332" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D333, "',",Players!A333, ",'",Players!E333,"','",Players!F333,"','",Players!G333,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A332" s="2"/>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A333" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D334, "',",Players!A334, ",'",Players!E334,"','",Players!F334,"','",Players!G334,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A333" s="2"/>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A334" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D335, "',",Players!A335, ",'",Players!E335,"','",Players!F335,"','",Players!G335,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A334" s="2"/>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D336, "',",Players!A336, ",'",Players!E336,"','",Players!F336,"','",Players!G336,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A335" s="2"/>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A336" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D337, "',",Players!A337, ",'",Players!E337,"','",Players!F337,"','",Players!G337,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A336" s="2"/>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D338, "',",Players!A338, ",'",Players!E338,"','",Players!F338,"','",Players!G338,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A337" s="2"/>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D339, "',",Players!A339, ",'",Players!E339,"','",Players!F339,"','",Players!G339,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A338" s="2"/>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A339" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D340, "',",Players!A340, ",'",Players!E340,"','",Players!F340,"','",Players!G340,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A339" s="2"/>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D341, "',",Players!A341, ",'",Players!E341,"','",Players!F341,"','",Players!G341,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A340" s="2"/>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D342, "',",Players!A342, ",'",Players!E342,"','",Players!F342,"','",Players!G342,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A341" s="2"/>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D343, "',",Players!A343, ",'",Players!E343,"','",Players!F343,"','",Players!G343,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A342" s="2"/>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D344, "',",Players!A344, ",'",Players!E344,"','",Players!F344,"','",Players!G344,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A343" s="2"/>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A344" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D345, "',",Players!A345, ",'",Players!E345,"','",Players!F345,"','",Players!G345,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A344" s="2"/>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D346, "',",Players!A346, ",'",Players!E346,"','",Players!F346,"','",Players!G346,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A345" s="2"/>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A346" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D347, "',",Players!A347, ",'",Players!E347,"','",Players!F347,"','",Players!G347,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A346" s="2"/>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D348, "',",Players!A348, ",'",Players!E348,"','",Players!F348,"','",Players!G348,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A347" s="2"/>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D349, "',",Players!A349, ",'",Players!E349,"','",Players!F349,"','",Players!G349,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A348" s="2"/>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A349" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D350, "',",Players!A350, ",'",Players!E350,"','",Players!F350,"','",Players!G350,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A349" s="2"/>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A350" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D351, "',",Players!A351, ",'",Players!E351,"','",Players!F351,"','",Players!G351,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A350" s="2"/>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A351" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D352, "',",Players!A352, ",'",Players!E352,"','",Players!F352,"','",Players!G352,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A351" s="2"/>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D353, "',",Players!A353, ",'",Players!E353,"','",Players!F353,"','",Players!G353,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A352" s="2"/>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A353" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D354, "',",Players!A354, ",'",Players!E354,"','",Players!F354,"','",Players!G354,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A353" s="2"/>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D355, "',",Players!A355, ",'",Players!E355,"','",Players!F355,"','",Players!G355,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A354" s="2"/>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A355" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D356, "',",Players!A356, ",'",Players!E356,"','",Players!F356,"','",Players!G356,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A355" s="2"/>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D357, "',",Players!A357, ",'",Players!E357,"','",Players!F357,"','",Players!G357,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A356" s="2"/>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A357" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D358, "',",Players!A358, ",'",Players!E358,"','",Players!F358,"','",Players!G358,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A357" s="2"/>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A358" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D359, "',",Players!A359, ",'",Players!E359,"','",Players!F359,"','",Players!G359,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A358" s="2"/>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A359" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D360, "',",Players!A360, ",'",Players!E360,"','",Players!F360,"','",Players!G360,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A359" s="2"/>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A360" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D361, "',",Players!A361, ",'",Players!E361,"','",Players!F361,"','",Players!G361,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A360" s="2"/>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D362, "',",Players!A362, ",'",Players!E362,"','",Players!F362,"','",Players!G362,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A361" s="2"/>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D363, "',",Players!A363, ",'",Players!E363,"','",Players!F363,"','",Players!G363,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A362" s="2"/>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D364, "',",Players!A364, ",'",Players!E364,"','",Players!F364,"','",Players!G364,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A363" s="2"/>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D365, "',",Players!A365, ",'",Players!E365,"','",Players!F365,"','",Players!G365,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A364" s="2"/>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D366, "',",Players!A366, ",'",Players!E366,"','",Players!F366,"','",Players!G366,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A365" s="2"/>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D367, "',",Players!A367, ",'",Players!E367,"','",Players!F367,"','",Players!G367,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A366" s="2"/>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D368, "',",Players!A368, ",'",Players!E368,"','",Players!F368,"','",Players!G368,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A367" s="2"/>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A368" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D369, "',",Players!A369, ",'",Players!E369,"','",Players!F369,"','",Players!G369,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A368" s="2"/>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D370, "',",Players!A370, ",'",Players!E370,"','",Players!F370,"','",Players!G370,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A369" s="2"/>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D371, "',",Players!A371, ",'",Players!E371,"','",Players!F371,"','",Players!G371,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A370" s="2"/>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D372, "',",Players!A372, ",'",Players!E372,"','",Players!F372,"','",Players!G372,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A371" s="2"/>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D373, "',",Players!A373, ",'",Players!E373,"','",Players!F373,"','",Players!G373,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A372" s="2"/>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D374, "',",Players!A374, ",'",Players!E374,"','",Players!F374,"','",Players!G374,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A373" s="2"/>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D375, "',",Players!A375, ",'",Players!E375,"','",Players!F375,"','",Players!G375,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A374" s="2"/>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D376, "',",Players!A376, ",'",Players!E376,"','",Players!F376,"','",Players!G376,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A375" s="2"/>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D377, "',",Players!A377, ",'",Players!E377,"','",Players!F377,"','",Players!G377,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A376" s="2"/>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D378, "',",Players!A378, ",'",Players!E378,"','",Players!F378,"','",Players!G378,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A377" s="2"/>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A378" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D379, "',",Players!A379, ",'",Players!E379,"','",Players!F379,"','",Players!G379,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A378" s="2"/>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A379" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D380, "',",Players!A380, ",'",Players!E380,"','",Players!F380,"','",Players!G380,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A379" s="2"/>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A380" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D381, "',",Players!A381, ",'",Players!E381,"','",Players!F381,"','",Players!G381,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A380" s="2"/>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A381" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D382, "',",Players!A382, ",'",Players!E382,"','",Players!F382,"','",Players!G382,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A381" s="2"/>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D383, "',",Players!A383, ",'",Players!E383,"','",Players!F383,"','",Players!G383,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A382" s="2"/>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D384, "',",Players!A384, ",'",Players!E384,"','",Players!F384,"','",Players!G384,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A383" s="2"/>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D385, "',",Players!A385, ",'",Players!E385,"','",Players!F385,"','",Players!G385,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A384" s="2"/>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A385" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D386, "',",Players!A386, ",'",Players!E386,"','",Players!F386,"','",Players!G386,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A385" s="2"/>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A386" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D387, "',",Players!A387, ",'",Players!E387,"','",Players!F387,"','",Players!G387,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A386" s="2"/>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D388, "',",Players!A388, ",'",Players!E388,"','",Players!F388,"','",Players!G388,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A387" s="2"/>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D389, "',",Players!A389, ",'",Players!E389,"','",Players!F389,"','",Players!G389,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A388" s="2"/>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D390, "',",Players!A390, ",'",Players!E390,"','",Players!F390,"','",Players!G390,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A389" s="2"/>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D391, "',",Players!A391, ",'",Players!E391,"','",Players!F391,"','",Players!G391,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A390" s="2"/>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A391" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D392, "',",Players!A392, ",'",Players!E392,"','",Players!F392,"','",Players!G392,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A391" s="2"/>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D393, "',",Players!A393, ",'",Players!E393,"','",Players!F393,"','",Players!G393,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A392" s="2"/>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A393" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D394, "',",Players!A394, ",'",Players!E394,"','",Players!F394,"','",Players!G394,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A393" s="2"/>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D395, "',",Players!A395, ",'",Players!E395,"','",Players!F395,"','",Players!G395,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A394" s="2"/>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A395" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D396, "',",Players!A396, ",'",Players!E396,"','",Players!F396,"','",Players!G396,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A395" s="2"/>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A396" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D397, "',",Players!A397, ",'",Players!E397,"','",Players!F397,"','",Players!G397,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A396" s="2"/>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A397" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D398, "',",Players!A398, ",'",Players!E398,"','",Players!F398,"','",Players!G398,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A397" s="2"/>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A398" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D399, "',",Players!A399, ",'",Players!E399,"','",Players!F399,"','",Players!G399,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A398" s="2"/>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A399" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D400, "',",Players!A400, ",'",Players!E400,"','",Players!F400,"','",Players!G400,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A399" s="2"/>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A400" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D401, "',",Players!A401, ",'",Players!E401,"','",Players!F401,"','",Players!G401,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A400" s="2"/>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A401" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D402, "',",Players!A402, ",'",Players!E402,"','",Players!F402,"','",Players!G402,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A401" s="2"/>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A402" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D403, "',",Players!A403, ",'",Players!E403,"','",Players!F403,"','",Players!G403,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A402" s="2"/>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D404, "',",Players!A404, ",'",Players!E404,"','",Players!F404,"','",Players!G404,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A403" s="2"/>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A404" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D405, "',",Players!A405, ",'",Players!E405,"','",Players!F405,"','",Players!G405,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A404" s="2"/>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D406, "',",Players!A406, ",'",Players!E406,"','",Players!F406,"','",Players!G406,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A405" s="2"/>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A406" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D407, "',",Players!A407, ",'",Players!E407,"','",Players!F407,"','",Players!G407,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A406" s="2"/>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A407" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D408, "',",Players!A408, ",'",Players!E408,"','",Players!F408,"','",Players!G408,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A407" s="2"/>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A408" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D409, "',",Players!A409, ",'",Players!E409,"','",Players!F409,"','",Players!G409,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A408" s="2"/>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A409" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D410, "',",Players!A410, ",'",Players!E410,"','",Players!F410,"','",Players!G410,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A409" s="2"/>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D411, "',",Players!A411, ",'",Players!E411,"','",Players!F411,"','",Players!G411,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A410" s="2"/>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D412, "',",Players!A412, ",'",Players!E412,"','",Players!F412,"','",Players!G412,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A411" s="2"/>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D413, "',",Players!A413, ",'",Players!E413,"','",Players!F413,"','",Players!G413,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A412" s="2"/>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D414, "',",Players!A414, ",'",Players!E414,"','",Players!F414,"','",Players!G414,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A413" s="2"/>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D415, "',",Players!A415, ",'",Players!E415,"','",Players!F415,"','",Players!G415,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A414" s="2"/>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A415" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D416, "',",Players!A416, ",'",Players!E416,"','",Players!F416,"','",Players!G416,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A415" s="2"/>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D417, "',",Players!A417, ",'",Players!E417,"','",Players!F417,"','",Players!G417,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A416" s="2"/>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D418, "',",Players!A418, ",'",Players!E418,"','",Players!F418,"','",Players!G418,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A417" s="2"/>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A418" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D419, "',",Players!A419, ",'",Players!E419,"','",Players!F419,"','",Players!G419,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A418" s="2"/>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D420, "',",Players!A420, ",'",Players!E420,"','",Players!F420,"','",Players!G420,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A419" s="2"/>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A420" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D421, "',",Players!A421, ",'",Players!E421,"','",Players!F421,"','",Players!G421,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A420" s="2"/>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D422, "',",Players!A422, ",'",Players!E422,"','",Players!F422,"','",Players!G422,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A421" s="2"/>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D423, "',",Players!A423, ",'",Players!E423,"','",Players!F423,"','",Players!G423,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A422" s="2"/>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D424, "',",Players!A424, ",'",Players!E424,"','",Players!F424,"','",Players!G424,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A423" s="2"/>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D425, "',",Players!A425, ",'",Players!E425,"','",Players!F425,"','",Players!G425,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A424" s="2"/>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D426, "',",Players!A426, ",'",Players!E426,"','",Players!F426,"','",Players!G426,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A425" s="2"/>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D427, "',",Players!A427, ",'",Players!E427,"','",Players!F427,"','",Players!G427,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A426" s="2"/>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A427" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D428, "',",Players!A428, ",'",Players!E428,"','",Players!F428,"','",Players!G428,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A427" s="2"/>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A428" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D429, "',",Players!A429, ",'",Players!E429,"','",Players!F429,"','",Players!G429,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A428" s="2"/>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A429" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D430, "',",Players!A430, ",'",Players!E430,"','",Players!F430,"','",Players!G430,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A429" s="2"/>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A430" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D431, "',",Players!A431, ",'",Players!E431,"','",Players!F431,"','",Players!G431,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A430" s="2"/>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A431" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D432, "',",Players!A432, ",'",Players!E432,"','",Players!F432,"','",Players!G432,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A431" s="2"/>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A432" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D433, "',",Players!A433, ",'",Players!E433,"','",Players!F433,"','",Players!G433,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A432" s="2"/>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A433" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D434, "',",Players!A434, ",'",Players!E434,"','",Players!F434,"','",Players!G434,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A433" s="2"/>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A434" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D435, "',",Players!A435, ",'",Players!E435,"','",Players!F435,"','",Players!G435,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A434" s="2"/>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A435" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D436, "',",Players!A436, ",'",Players!E436,"','",Players!F436,"','",Players!G436,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A435" s="2"/>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A436" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D437, "',",Players!A437, ",'",Players!E437,"','",Players!F437,"','",Players!G437,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A436" s="2"/>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A437" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D438, "',",Players!A438, ",'",Players!E438,"','",Players!F438,"','",Players!G438,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A437" s="2"/>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A438" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D439, "',",Players!A439, ",'",Players!E439,"','",Players!F439,"','",Players!G439,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A438" s="2"/>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A439" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D440, "',",Players!A440, ",'",Players!E440,"','",Players!F440,"','",Players!G440,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A439" s="2"/>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A440" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D441, "',",Players!A441, ",'",Players!E441,"','",Players!F441,"','",Players!G441,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A440" s="2"/>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A441" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D442, "',",Players!A442, ",'",Players!E442,"','",Players!F442,"','",Players!G442,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A441" s="2"/>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D443, "',",Players!A443, ",'",Players!E443,"','",Players!F443,"','",Players!G443,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A442" s="2"/>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D444, "',",Players!A444, ",'",Players!E444,"','",Players!F444,"','",Players!G444,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A443" s="2"/>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D445, "',",Players!A445, ",'",Players!E445,"','",Players!F445,"','",Players!G445,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A444" s="2"/>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D446, "',",Players!A446, ",'",Players!E446,"','",Players!F446,"','",Players!G446,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A445" s="2"/>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D447, "',",Players!A447, ",'",Players!E447,"','",Players!F447,"','",Players!G447,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A446" s="2"/>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A447" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D448, "',",Players!A448, ",'",Players!E448,"','",Players!F448,"','",Players!G448,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A447" s="2"/>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D449, "',",Players!A449, ",'",Players!E449,"','",Players!F449,"','",Players!G449,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A448" s="2"/>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D450, "',",Players!A450, ",'",Players!E450,"','",Players!F450,"','",Players!G450,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A449" s="2"/>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D451, "',",Players!A451, ",'",Players!E451,"','",Players!F451,"','",Players!G451,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A450" s="2"/>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A451" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D452, "',",Players!A452, ",'",Players!E452,"','",Players!F452,"','",Players!G452,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A451" s="2"/>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D453, "',",Players!A453, ",'",Players!E453,"','",Players!F453,"','",Players!G453,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A452" s="2"/>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A453" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D454, "',",Players!A454, ",'",Players!E454,"','",Players!F454,"','",Players!G454,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A453" s="2"/>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A454" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D455, "',",Players!A455, ",'",Players!E455,"','",Players!F455,"','",Players!G455,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A454" s="2"/>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A455" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D456, "',",Players!A456, ",'",Players!E456,"','",Players!F456,"','",Players!G456,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A455" s="2"/>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A456" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D457, "',",Players!A457, ",'",Players!E457,"','",Players!F457,"','",Players!G457,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A456" s="2"/>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A457" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D458, "',",Players!A458, ",'",Players!E458,"','",Players!F458,"','",Players!G458,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A457" s="2"/>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A458" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D459, "',",Players!A459, ",'",Players!E459,"','",Players!F459,"','",Players!G459,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A458" s="2"/>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A459" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D460, "',",Players!A460, ",'",Players!E460,"','",Players!F460,"','",Players!G460,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A459" s="2"/>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A460" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D461, "',",Players!A461, ",'",Players!E461,"','",Players!F461,"','",Players!G461,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A460" s="2"/>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A461" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D462, "',",Players!A462, ",'",Players!E462,"','",Players!F462,"','",Players!G462,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A461" s="2"/>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A462" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D463, "',",Players!A463, ",'",Players!E463,"','",Players!F463,"','",Players!G463,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A462" s="2"/>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A463" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D464, "',",Players!A464, ",'",Players!E464,"','",Players!F464,"','",Players!G464,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A463" s="2"/>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A464" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D465, "',",Players!A465, ",'",Players!E465,"','",Players!F465,"','",Players!G465,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A464" s="2"/>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A465" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D466, "',",Players!A466, ",'",Players!E466,"','",Players!F466,"','",Players!G466,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A465" s="2"/>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A466" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D467, "',",Players!A467, ",'",Players!E467,"','",Players!F467,"','",Players!G467,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A466" s="2"/>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A467" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D468, "',",Players!A468, ",'",Players!E468,"','",Players!F468,"','",Players!G468,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A467" s="2"/>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A468" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D469, "',",Players!A469, ",'",Players!E469,"','",Players!F469,"','",Players!G469,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A468" s="2"/>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A469" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D470, "',",Players!A470, ",'",Players!E470,"','",Players!F470,"','",Players!G470,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A469" s="2"/>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A470" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D471, "',",Players!A471, ",'",Players!E471,"','",Players!F471,"','",Players!G471,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A470" s="2"/>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A471" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D472, "',",Players!A472, ",'",Players!E472,"','",Players!F472,"','",Players!G472,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A471" s="2"/>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A472" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D473, "',",Players!A473, ",'",Players!E473,"','",Players!F473,"','",Players!G473,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A472" s="2"/>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A473" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D474, "',",Players!A474, ",'",Players!E474,"','",Players!F474,"','",Players!G474,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A473" s="2"/>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A474" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D475, "',",Players!A475, ",'",Players!E475,"','",Players!F475,"','",Players!G475,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A474" s="2"/>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D476, "',",Players!A476, ",'",Players!E476,"','",Players!F476,"','",Players!G476,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A475" s="2"/>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A476" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D477, "',",Players!A477, ",'",Players!E477,"','",Players!F477,"','",Players!G477,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A476" s="2"/>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A477" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D478, "',",Players!A478, ",'",Players!E478,"','",Players!F478,"','",Players!G478,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A477" s="2"/>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A478" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D479, "',",Players!A479, ",'",Players!E479,"','",Players!F479,"','",Players!G479,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A478" s="2"/>
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A479" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D480, "',",Players!A480, ",'",Players!E480,"','",Players!F480,"','",Players!G480,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A479" s="2"/>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A480" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D481, "',",Players!A481, ",'",Players!E481,"','",Players!F481,"','",Players!G481,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A480" s="2"/>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A481" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D482, "',",Players!A482, ",'",Players!E482,"','",Players!F482,"','",Players!G482,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A481" s="2"/>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A482" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D483, "',",Players!A483, ",'",Players!E483,"','",Players!F483,"','",Players!G483,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A482" s="2"/>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A483" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D484, "',",Players!A484, ",'",Players!E484,"','",Players!F484,"','",Players!G484,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A483" s="2"/>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A484" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D485, "',",Players!A485, ",'",Players!E485,"','",Players!F485,"','",Players!G485,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A484" s="2"/>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A485" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D486, "',",Players!A486, ",'",Players!E486,"','",Players!F486,"','",Players!G486,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A485" s="2"/>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A486" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D487, "',",Players!A487, ",'",Players!E487,"','",Players!F487,"','",Players!G487,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A486" s="2"/>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A487" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D488, "',",Players!A488, ",'",Players!E488,"','",Players!F488,"','",Players!G488,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A487" s="2"/>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A488" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D489, "',",Players!A489, ",'",Players!E489,"','",Players!F489,"','",Players!G489,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A488" s="2"/>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A489" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D490, "',",Players!A490, ",'",Players!E490,"','",Players!F490,"','",Players!G490,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A489" s="2"/>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A490" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D491, "',",Players!A491, ",'",Players!E491,"','",Players!F491,"','",Players!G491,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A490" s="2"/>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A491" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D492, "',",Players!A492, ",'",Players!E492,"','",Players!F492,"','",Players!G492,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A491" s="2"/>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A492" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D493, "',",Players!A493, ",'",Players!E493,"','",Players!F493,"','",Players!G493,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A492" s="2"/>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A493" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D494, "',",Players!A494, ",'",Players!E494,"','",Players!F494,"','",Players!G494,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A493" s="2"/>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A494" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D495, "',",Players!A495, ",'",Players!E495,"','",Players!F495,"','",Players!G495,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A494" s="2"/>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A495" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D496, "',",Players!A496, ",'",Players!E496,"','",Players!F496,"','",Players!G496,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A495" s="2"/>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A496" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D497, "',",Players!A497, ",'",Players!E497,"','",Players!F497,"','",Players!G497,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A496" s="2"/>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A497" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D498, "',",Players!A498, ",'",Players!E498,"','",Players!F498,"','",Players!G498,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A497" s="2"/>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A498" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D499, "',",Players!A499, ",'",Players!E499,"','",Players!F499,"','",Players!G499,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A498" s="2"/>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A499" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D500, "',",Players!A500, ",'",Players!E500,"','",Players!F500,"','",Players!G500,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A499" s="2"/>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A500" s="2" t="str">
-        <f>_xlfn.CONCAT( "Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('", Players!D501, "',",Players!A501, ",'",Players!E501,"','",Players!F501,"','",Players!G501,"')")</f>
-        <v>Insert into topFCPlayerList (playerName, playerNumber, tryoutDate, playerAgeGroup, playerGender) VALUES ('',,'','','')</v>
-      </c>
+      <c r="A500" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>